<commit_message>
done test filter stock
</commit_message>
<xml_diff>
--- a/xlsx_data/full_stock_classification.xlsx
+++ b/xlsx_data/full_stock_classification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\t2m-project\t2m-python-v2\xlsx_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325BEA7F-8C72-403C-ADB3-2A8E9EC0F6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263C6914-1B02-4FB5-87CB-A40484467F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="period_stock_list" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17037" uniqueCount="1757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16688" uniqueCount="1757">
   <si>
     <t>PGC</t>
   </si>
@@ -31283,9 +31283,9 @@
         <f>VLOOKUP(D10,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10" t="e">
         <f>VLOOKUP(A10,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -31399,9 +31399,9 @@
         <f>VLOOKUP(D14,name_map!$A$2:$D$32,3,0)</f>
         <v>Dệt may</v>
       </c>
-      <c r="G14" t="e">
+      <c r="G14" t="str">
         <f>VLOOKUP(A14,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -31486,9 +31486,9 @@
         <f>VLOOKUP(D17,name_map!$A$2:$D$32,3,0)</f>
         <v>Thép</v>
       </c>
-      <c r="G17" t="str">
+      <c r="G17" t="e">
         <f>VLOOKUP(A17,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -31631,9 +31631,9 @@
         <f>VLOOKUP(D22,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G22" t="e">
+      <c r="G22" t="str">
         <f>VLOOKUP(A22,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -32356,9 +32356,9 @@
         <f>VLOOKUP(D47,name_map!$A$2:$D$32,3,0)</f>
         <v>Chứng khoán</v>
       </c>
-      <c r="G47" t="str">
+      <c r="G47" t="e">
         <f>VLOOKUP(A47,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -32646,9 +32646,9 @@
         <f>VLOOKUP(D57,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G57" t="str">
+      <c r="G57" t="e">
         <f>VLOOKUP(A57,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -32849,9 +32849,9 @@
         <f>VLOOKUP(D64,name_map!$A$2:$D$32,3,0)</f>
         <v>BĐS KCN</v>
       </c>
-      <c r="G64" t="e">
+      <c r="G64" t="str">
         <f>VLOOKUP(A64,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -32907,9 +32907,9 @@
         <f>VLOOKUP(D66,name_map!$A$2:$D$32,3,0)</f>
         <v>Xây dựng</v>
       </c>
-      <c r="G66" t="str">
+      <c r="G66" t="e">
         <f>VLOOKUP(A66,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -33197,9 +33197,9 @@
         <f>VLOOKUP(D76,name_map!$A$2:$D$32,3,0)</f>
         <v>BĐS KCN</v>
       </c>
-      <c r="G76" t="e">
+      <c r="G76" t="str">
         <f>VLOOKUP(A76,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -33284,9 +33284,9 @@
         <f>VLOOKUP(D79,name_map!$A$2:$D$32,3,0)</f>
         <v>Dệt may</v>
       </c>
-      <c r="G79" t="e">
+      <c r="G79" t="str">
         <f>VLOOKUP(A79,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -33342,9 +33342,9 @@
         <f>VLOOKUP(D81,name_map!$A$2:$D$32,3,0)</f>
         <v>Dầu khí</v>
       </c>
-      <c r="G81" t="e">
+      <c r="G81" t="str">
         <f>VLOOKUP(A81,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -33516,9 +33516,9 @@
         <f>VLOOKUP(D87,name_map!$A$2:$D$32,3,0)</f>
         <v>Xây dựng</v>
       </c>
-      <c r="G87" t="str">
+      <c r="G87" t="e">
         <f>VLOOKUP(A87,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -33574,9 +33574,9 @@
         <f>VLOOKUP(D89,name_map!$A$2:$D$32,3,0)</f>
         <v>Xây dựng</v>
       </c>
-      <c r="G89" t="str">
+      <c r="G89" t="e">
         <f>VLOOKUP(A89,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -33690,9 +33690,9 @@
         <f>VLOOKUP(D93,name_map!$A$2:$D$32,3,0)</f>
         <v>BĐS KCN</v>
       </c>
-      <c r="G93" t="e">
+      <c r="G93" t="str">
         <f>VLOOKUP(A93,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -33748,9 +33748,9 @@
         <f>VLOOKUP(D95,name_map!$A$2:$D$32,3,0)</f>
         <v>Khoáng sản</v>
       </c>
-      <c r="G95" t="e">
+      <c r="G95" t="str">
         <f>VLOOKUP(A95,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -34009,9 +34009,9 @@
         <f>VLOOKUP(D104,name_map!$A$2:$D$32,3,0)</f>
         <v>Du lịch và DV</v>
       </c>
-      <c r="G104" t="str">
+      <c r="G104" t="e">
         <f>VLOOKUP(A104,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -34415,9 +34415,9 @@
         <f>VLOOKUP(D118,name_map!$A$2:$D$32,3,0)</f>
         <v>Thực phẩm</v>
       </c>
-      <c r="G118" t="e">
+      <c r="G118" t="str">
         <f>VLOOKUP(A118,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -34763,9 +34763,9 @@
         <f>VLOOKUP(D130,name_map!$A$2:$D$32,3,0)</f>
         <v>Vận tải</v>
       </c>
-      <c r="G130" t="str">
+      <c r="G130" t="e">
         <f>VLOOKUP(A130,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -34966,9 +34966,9 @@
         <f>VLOOKUP(D137,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G137" t="str">
+      <c r="G137" t="e">
         <f>VLOOKUP(A137,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -34995,9 +34995,9 @@
         <f>VLOOKUP(D138,name_map!$A$2:$D$32,3,0)</f>
         <v>Xây dựng</v>
       </c>
-      <c r="G138" t="e">
+      <c r="G138" t="str">
         <f>VLOOKUP(A138,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -35285,9 +35285,9 @@
         <f>VLOOKUP(D148,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G148" t="e">
+      <c r="G148" t="str">
         <f>VLOOKUP(A148,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -35517,9 +35517,9 @@
         <f>VLOOKUP(D156,name_map!$A$2:$D$32,3,0)</f>
         <v>Thực phẩm</v>
       </c>
-      <c r="G156" t="e">
+      <c r="G156" t="str">
         <f>VLOOKUP(A156,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -35546,9 +35546,9 @@
         <f>VLOOKUP(D157,name_map!$A$2:$D$32,3,0)</f>
         <v>Công nghệ</v>
       </c>
-      <c r="G157" t="str">
+      <c r="G157" t="e">
         <f>VLOOKUP(A157,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -36010,9 +36010,9 @@
         <f>VLOOKUP(D173,name_map!$A$2:$D$32,3,0)</f>
         <v>BĐS KCN</v>
       </c>
-      <c r="G173" t="e">
+      <c r="G173" t="str">
         <f>VLOOKUP(A173,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -36155,9 +36155,9 @@
         <f>VLOOKUP(D178,name_map!$A$2:$D$32,3,0)</f>
         <v>Công nghệ</v>
       </c>
-      <c r="G178" t="str">
+      <c r="G178" t="e">
         <f>VLOOKUP(A178,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -37170,9 +37170,9 @@
         <f>VLOOKUP(D213,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G213" t="e">
+      <c r="G213" t="str">
         <f>VLOOKUP(A213,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -37286,9 +37286,9 @@
         <f>VLOOKUP(D217,name_map!$A$2:$D$32,3,0)</f>
         <v>Xây dựng</v>
       </c>
-      <c r="G217" t="str">
+      <c r="G217" t="e">
         <f>VLOOKUP(A217,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -37692,9 +37692,9 @@
         <f>VLOOKUP(D231,name_map!$A$2:$D$32,3,0)</f>
         <v>BĐS KCN</v>
       </c>
-      <c r="G231" t="e">
+      <c r="G231" t="str">
         <f>VLOOKUP(A231,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -38562,9 +38562,9 @@
         <f>VLOOKUP(D261,name_map!$A$2:$D$32,3,0)</f>
         <v>BĐS KCN</v>
       </c>
-      <c r="G261" t="e">
+      <c r="G261" t="str">
         <f>VLOOKUP(A261,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
@@ -39113,9 +39113,9 @@
         <f>VLOOKUP(D280,name_map!$A$2:$D$32,3,0)</f>
         <v>Vận tải</v>
       </c>
-      <c r="G280" t="e">
+      <c r="G280" t="str">
         <f>VLOOKUP(A280,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -39287,9 +39287,9 @@
         <f>VLOOKUP(D286,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G286" t="e">
+      <c r="G286" t="str">
         <f>VLOOKUP(A286,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
@@ -39374,9 +39374,9 @@
         <f>VLOOKUP(D289,name_map!$A$2:$D$32,3,0)</f>
         <v>Chứng khoán</v>
       </c>
-      <c r="G289" t="str">
+      <c r="G289" t="e">
         <f>VLOOKUP(A289,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
@@ -40186,9 +40186,9 @@
         <f>VLOOKUP(D317,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G317" t="str">
+      <c r="G317" t="e">
         <f>VLOOKUP(A317,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
@@ -40215,9 +40215,9 @@
         <f>VLOOKUP(D318,name_map!$A$2:$D$32,3,0)</f>
         <v>Xây dựng</v>
       </c>
-      <c r="G318" t="e">
+      <c r="G318" t="str">
         <f>VLOOKUP(A318,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.25">
@@ -40273,9 +40273,9 @@
         <f>VLOOKUP(D320,name_map!$A$2:$D$32,3,0)</f>
         <v>Thực phẩm</v>
       </c>
-      <c r="G320" t="e">
+      <c r="G320" t="str">
         <f>VLOOKUP(A320,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.25">
@@ -40360,9 +40360,9 @@
         <f>VLOOKUP(D323,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G323" t="str">
+      <c r="G323" t="e">
         <f>VLOOKUP(A323,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.25">
@@ -40447,9 +40447,9 @@
         <f>VLOOKUP(D326,name_map!$A$2:$D$32,3,0)</f>
         <v>Vận tải</v>
       </c>
-      <c r="G326" t="e">
+      <c r="G326" t="str">
         <f>VLOOKUP(A326,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.25">
@@ -40534,9 +40534,9 @@
         <f>VLOOKUP(D329,name_map!$A$2:$D$32,3,0)</f>
         <v>Thực phẩm</v>
       </c>
-      <c r="G329" t="str">
+      <c r="G329" t="e">
         <f>VLOOKUP(A329,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.25">
@@ -41345,9 +41345,9 @@
         <f>VLOOKUP(D357,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G357" t="str">
+      <c r="G357" t="e">
         <f>VLOOKUP(A357,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="358" spans="1:7" x14ac:dyDescent="0.25">
@@ -41722,9 +41722,9 @@
         <f>VLOOKUP(D370,name_map!$A$2:$D$32,3,0)</f>
         <v>Dệt may</v>
       </c>
-      <c r="G370" t="e">
+      <c r="G370" t="str">
         <f>VLOOKUP(A370,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
@@ -41954,9 +41954,9 @@
         <f>VLOOKUP(D378,name_map!$A$2:$D$32,3,0)</f>
         <v>Dầu khí</v>
       </c>
-      <c r="G378" t="str">
+      <c r="G378" t="e">
         <f>VLOOKUP(A378,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
@@ -41983,9 +41983,9 @@
         <f>VLOOKUP(D379,name_map!$A$2:$D$32,3,0)</f>
         <v>Vận tải</v>
       </c>
-      <c r="G379" t="e">
+      <c r="G379" t="str">
         <f>VLOOKUP(A379,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.25">
@@ -42099,9 +42099,9 @@
         <f>VLOOKUP(D383,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G383" t="e">
+      <c r="G383" t="str">
         <f>VLOOKUP(A383,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.25">
@@ -42823,9 +42823,9 @@
         <f>VLOOKUP(D408,name_map!$A$2:$D$32,3,0)</f>
         <v>Công nghiệp</v>
       </c>
-      <c r="G408" t="e">
+      <c r="G408" t="str">
         <f>VLOOKUP(A408,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.25">
@@ -43026,9 +43026,9 @@
         <f>VLOOKUP(D415,name_map!$A$2:$D$32,3,0)</f>
         <v>Công nghệ</v>
       </c>
-      <c r="G415" t="str">
+      <c r="G415" t="e">
         <f>VLOOKUP(A415,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="416" spans="1:7" x14ac:dyDescent="0.25">
@@ -43113,9 +43113,9 @@
         <f>VLOOKUP(D418,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G418" t="e">
+      <c r="G418" t="str">
         <f>VLOOKUP(A418,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="419" spans="1:7" x14ac:dyDescent="0.25">
@@ -43896,9 +43896,9 @@
         <f>VLOOKUP(D445,name_map!$A$2:$D$32,3,0)</f>
         <v>Dầu khí</v>
       </c>
-      <c r="G445" t="str">
+      <c r="G445" t="e">
         <f>VLOOKUP(A445,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.25">
@@ -44302,9 +44302,9 @@
         <f>VLOOKUP(D459,name_map!$A$2:$D$32,3,0)</f>
         <v>Ngân hàng</v>
       </c>
-      <c r="G459" t="e">
+      <c r="G459" t="str">
         <f>VLOOKUP(A459,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="460" spans="1:7" x14ac:dyDescent="0.25">
@@ -44389,9 +44389,9 @@
         <f>VLOOKUP(D462,name_map!$A$2:$D$32,3,0)</f>
         <v>Công ty tài chính</v>
       </c>
-      <c r="G462" t="e">
+      <c r="G462" t="str">
         <f>VLOOKUP(A462,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="463" spans="1:7" x14ac:dyDescent="0.25">
@@ -44418,9 +44418,9 @@
         <f>VLOOKUP(D463,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G463" t="str">
+      <c r="G463" t="e">
         <f>VLOOKUP(A463,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.25">
@@ -44534,9 +44534,9 @@
         <f>VLOOKUP(D467,name_map!$A$2:$D$32,3,0)</f>
         <v>Thép</v>
       </c>
-      <c r="G467" t="e">
+      <c r="G467" t="str">
         <f>VLOOKUP(A467,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="468" spans="1:7" x14ac:dyDescent="0.25">
@@ -44766,9 +44766,9 @@
         <f>VLOOKUP(D475,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G475" t="e">
+      <c r="G475" t="str">
         <f>VLOOKUP(A475,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="476" spans="1:7" x14ac:dyDescent="0.25">
@@ -44824,9 +44824,9 @@
         <f>VLOOKUP(D477,name_map!$A$2:$D$32,3,0)</f>
         <v>Ngân hàng</v>
       </c>
-      <c r="G477" t="str">
+      <c r="G477" t="e">
         <f>VLOOKUP(A477,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="478" spans="1:7" x14ac:dyDescent="0.25">
@@ -45317,9 +45317,9 @@
         <f>VLOOKUP(D494,name_map!$A$2:$D$32,3,0)</f>
         <v>Xây dựng</v>
       </c>
-      <c r="G494" t="str">
+      <c r="G494" t="e">
         <f>VLOOKUP(A494,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.25">
@@ -45491,9 +45491,9 @@
         <f>VLOOKUP(D500,name_map!$A$2:$D$32,3,0)</f>
         <v>Chứng khoán</v>
       </c>
-      <c r="G500" t="str">
+      <c r="G500" t="e">
         <f>VLOOKUP(A500,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="501" spans="1:7" x14ac:dyDescent="0.25">
@@ -45723,9 +45723,9 @@
         <f>VLOOKUP(D508,name_map!$A$2:$D$32,3,0)</f>
         <v>Hàng tiêu dùng</v>
       </c>
-      <c r="G508" t="e">
+      <c r="G508" t="str">
         <f>VLOOKUP(A508,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="509" spans="1:7" x14ac:dyDescent="0.25">
@@ -45810,9 +45810,9 @@
         <f>VLOOKUP(D511,name_map!$A$2:$D$32,3,0)</f>
         <v>BĐS KCN</v>
       </c>
-      <c r="G511" t="e">
+      <c r="G511" t="str">
         <f>VLOOKUP(A511,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.25">
@@ -46071,9 +46071,9 @@
         <f>VLOOKUP(D520,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G520" t="e">
+      <c r="G520" t="str">
         <f>VLOOKUP(A520,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="521" spans="1:7" x14ac:dyDescent="0.25">
@@ -46390,9 +46390,9 @@
         <f>VLOOKUP(D531,name_map!$A$2:$D$32,3,0)</f>
         <v>Xây dựng</v>
       </c>
-      <c r="G531" t="e">
+      <c r="G531" t="str">
         <f>VLOOKUP(A531,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="532" spans="1:7" x14ac:dyDescent="0.25">
@@ -46593,9 +46593,9 @@
         <f>VLOOKUP(D538,name_map!$A$2:$D$32,3,0)</f>
         <v>Hàng tiêu dùng</v>
       </c>
-      <c r="G538" t="e">
+      <c r="G538" t="str">
         <f>VLOOKUP(A538,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="539" spans="1:7" x14ac:dyDescent="0.25">
@@ -46767,9 +46767,9 @@
         <f>VLOOKUP(D544,name_map!$A$2:$D$32,3,0)</f>
         <v>Ngân hàng</v>
       </c>
-      <c r="G544" t="e">
+      <c r="G544" t="str">
         <f>VLOOKUP(A544,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="545" spans="1:7" x14ac:dyDescent="0.25">
@@ -46825,9 +46825,9 @@
         <f>VLOOKUP(D546,name_map!$A$2:$D$32,3,0)</f>
         <v>Chứng khoán</v>
       </c>
-      <c r="G546" t="str">
+      <c r="G546" t="e">
         <f>VLOOKUP(A546,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="547" spans="1:7" x14ac:dyDescent="0.25">
@@ -47521,9 +47521,9 @@
         <f>VLOOKUP(D570,name_map!$A$2:$D$32,3,0)</f>
         <v>Thực phẩm</v>
       </c>
-      <c r="G570" t="e">
+      <c r="G570" t="str">
         <f>VLOOKUP(A570,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.25">
@@ -47608,9 +47608,9 @@
         <f>VLOOKUP(D573,name_map!$A$2:$D$32,3,0)</f>
         <v>Công nghiệp</v>
       </c>
-      <c r="G573" t="str">
+      <c r="G573" t="e">
         <f>VLOOKUP(A573,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
@@ -47782,9 +47782,9 @@
         <f>VLOOKUP(D579,name_map!$A$2:$D$32,3,0)</f>
         <v>Công ty tài chính</v>
       </c>
-      <c r="G579" t="e">
+      <c r="G579" t="str">
         <f>VLOOKUP(A579,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="580" spans="1:7" x14ac:dyDescent="0.25">
@@ -47927,9 +47927,9 @@
         <f>VLOOKUP(D584,name_map!$A$2:$D$32,3,0)</f>
         <v>Thực phẩm</v>
       </c>
-      <c r="G584" t="str">
+      <c r="G584" t="e">
         <f>VLOOKUP(A584,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.25">
@@ -47956,9 +47956,9 @@
         <f>VLOOKUP(D585,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G585" t="e">
+      <c r="G585" t="str">
         <f>VLOOKUP(A585,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.25">
@@ -48246,9 +48246,9 @@
         <f>VLOOKUP(D595,name_map!$A$2:$D$32,3,0)</f>
         <v>Khoáng sản</v>
       </c>
-      <c r="G595" t="e">
+      <c r="G595" t="str">
         <f>VLOOKUP(A595,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.25">
@@ -48507,9 +48507,9 @@
         <f>VLOOKUP(D604,name_map!$A$2:$D$32,3,0)</f>
         <v>Hoá chất</v>
       </c>
-      <c r="G604" t="str">
+      <c r="G604" t="e">
         <f>VLOOKUP(A604,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.25">
@@ -48565,9 +48565,9 @@
         <f>VLOOKUP(D606,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G606" t="str">
+      <c r="G606" t="e">
         <f>VLOOKUP(A606,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="607" spans="1:7" x14ac:dyDescent="0.25">
@@ -49145,9 +49145,9 @@
         <f>VLOOKUP(D626,name_map!$A$2:$D$32,3,0)</f>
         <v>Ngân hàng</v>
       </c>
-      <c r="G626" t="str">
+      <c r="G626" t="e">
         <f>VLOOKUP(A626,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="627" spans="1:7" x14ac:dyDescent="0.25">
@@ -49348,9 +49348,9 @@
         <f>VLOOKUP(D633,name_map!$A$2:$D$32,3,0)</f>
         <v>Công ty tài chính</v>
       </c>
-      <c r="G633" t="e">
+      <c r="G633" t="str">
         <f>VLOOKUP(A633,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="634" spans="1:7" x14ac:dyDescent="0.25">
@@ -49377,9 +49377,9 @@
         <f>VLOOKUP(D634,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G634" t="str">
+      <c r="G634" t="e">
         <f>VLOOKUP(A634,signal_stock!$A:$B,2,)</f>
-        <v>x</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.25">
@@ -49638,9 +49638,9 @@
         <f>VLOOKUP(D643,name_map!$A$2:$D$32,3,0)</f>
         <v>Dệt may</v>
       </c>
-      <c r="G643" t="e">
+      <c r="G643" t="str">
         <f>VLOOKUP(A643,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.25">
@@ -49667,9 +49667,9 @@
         <f>VLOOKUP(D644,name_map!$A$2:$D$32,3,0)</f>
         <v>Bất động sản</v>
       </c>
-      <c r="G644" t="e">
+      <c r="G644" t="str">
         <f>VLOOKUP(A644,signal_stock!$A:$B,2,)</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
     </row>
     <row r="645" spans="1:7" x14ac:dyDescent="0.25">
@@ -81206,7 +81206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC4401C-D304-4750-8CED-A9CF758C9679}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -81673,3024 +81673,1977 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD58B990-4E93-4226-B2C3-FA35F0465DC7}">
-  <dimension ref="A1:F593"/>
+  <dimension ref="A1:B593"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>290</v>
+        <v>510</v>
       </c>
       <c r="B1" t="str">
         <f t="shared" ref="B1:B32" si="0">IF(LEN(A1)=3, "x", " ")</f>
         <v>x</v>
       </c>
-      <c r="E1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>418</v>
+        <v>215</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E2" t="s">
-        <v>418</v>
-      </c>
-      <c r="F2" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>560</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>309</v>
+        <v>628</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E5" t="s">
-        <v>309</v>
-      </c>
-      <c r="F5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>540</v>
+        <v>303</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E6" t="s">
-        <v>540</v>
-      </c>
-      <c r="F6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>307</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F7" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>586</v>
+        <v>140</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E8" t="s">
-        <v>586</v>
-      </c>
-      <c r="F8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>225</v>
+        <v>496</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E10" t="s">
-        <v>225</v>
-      </c>
-      <c r="F10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>291</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>173</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>271</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F13" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>351</v>
+        <v>107</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E14" t="s">
-        <v>351</v>
-      </c>
-      <c r="F14" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>383</v>
+        <v>294</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E15" t="s">
-        <v>383</v>
-      </c>
-      <c r="F15" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>359</v>
+        <v>185</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E16" t="s">
-        <v>359</v>
-      </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E17" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>608</v>
+        <v>351</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E18" t="s">
-        <v>608</v>
-      </c>
-      <c r="F18" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>9</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E19" t="s">
-        <v>169</v>
-      </c>
-      <c r="F19" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>519</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E20" t="s">
-        <v>173</v>
-      </c>
-      <c r="F20" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E21" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>193</v>
-      </c>
-      <c r="F21" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>622</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>622</v>
-      </c>
-      <c r="F22" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>261</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E23" t="s">
-        <v>261</v>
-      </c>
-      <c r="F23" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>522</v>
+        <v>492</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E24" t="s">
-        <v>522</v>
-      </c>
-      <c r="F24" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>367</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>492</v>
+        <v>110</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E26" t="s">
-        <v>492</v>
-      </c>
-      <c r="F26" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>376</v>
+        <v>38</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E27" t="s">
-        <v>376</v>
-      </c>
-      <c r="F27" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E28" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>519</v>
+        <v>295</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E29" t="s">
-        <v>519</v>
-      </c>
-      <c r="F29" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>501</v>
+        <v>272</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E30" t="s">
-        <v>501</v>
-      </c>
-      <c r="F30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>307</v>
+        <v>149</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E31" t="s">
-        <v>307</v>
-      </c>
-      <c r="F31" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>448</v>
+        <v>83</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="E32" t="s">
-        <v>448</v>
-      </c>
-      <c r="F32" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>572</v>
+        <v>522</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" ref="B33:B96" si="1">IF(LEN(A33)=3, "x", " ")</f>
         <v>x</v>
       </c>
-      <c r="E33" t="s">
-        <v>572</v>
-      </c>
-      <c r="F33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>526</v>
+        <v>608</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E34" t="s">
-        <v>322</v>
-      </c>
-      <c r="F34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>20</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E35" t="s">
-        <v>526</v>
-      </c>
-      <c r="F35" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>400</v>
+        <v>281</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E36" t="s">
-        <v>185</v>
-      </c>
-      <c r="F36" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>294</v>
+        <v>202</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E37" t="s">
-        <v>400</v>
-      </c>
-      <c r="F37" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>159</v>
+        <v>397</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E38" t="s">
-        <v>294</v>
-      </c>
-      <c r="F38" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>559</v>
+        <v>76</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E39" t="s">
-        <v>159</v>
-      </c>
-      <c r="F39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>472</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E40" t="s">
-        <v>559</v>
-      </c>
-      <c r="F40" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>558</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E41" t="s">
-        <v>89</v>
-      </c>
-      <c r="F41" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>376</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E42" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>222</v>
+        <v>359</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E44" t="s">
-        <v>222</v>
-      </c>
-      <c r="F44" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>386</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E45" t="s">
-        <v>271</v>
-      </c>
-      <c r="F45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>462</v>
+        <v>401</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E46" t="s">
-        <v>194</v>
-      </c>
-      <c r="F46" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>409</v>
+        <v>609</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E47" t="s">
-        <v>462</v>
-      </c>
-      <c r="F47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E48" t="s">
-        <v>409</v>
-      </c>
-      <c r="F48" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>367</v>
+        <v>256</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E49" t="s">
-        <v>107</v>
-      </c>
-      <c r="F49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>576</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E50" t="s">
-        <v>367</v>
-      </c>
-      <c r="F50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>630</v>
+        <v>226</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E51" t="s">
-        <v>65</v>
-      </c>
-      <c r="F51" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E52" t="s">
-        <v>630</v>
-      </c>
-      <c r="F52" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>612</v>
+        <v>498</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E53" t="s">
-        <v>30</v>
-      </c>
-      <c r="F53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>143</v>
+        <v>497</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E54" t="s">
-        <v>612</v>
-      </c>
-      <c r="F54" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>625</v>
+        <v>122</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E55" t="s">
-        <v>143</v>
-      </c>
-      <c r="F55" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>199</v>
+        <v>72</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E56" t="s">
-        <v>625</v>
-      </c>
-      <c r="F56" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>437</v>
+        <v>374</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E57" t="s">
-        <v>199</v>
-      </c>
-      <c r="F57" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>576</v>
+        <v>172</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E58" t="s">
-        <v>437</v>
-      </c>
-      <c r="F58" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>401</v>
+        <v>277</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E59" t="s">
-        <v>576</v>
-      </c>
-      <c r="F59" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>618</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E60" t="s">
-        <v>401</v>
-      </c>
-      <c r="F60" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>551</v>
+        <v>27</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E61" t="s">
-        <v>35</v>
-      </c>
-      <c r="F61" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>332</v>
+        <v>437</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E62" t="s">
-        <v>551</v>
-      </c>
-      <c r="F62" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>599</v>
+        <v>487</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E63" t="s">
-        <v>332</v>
-      </c>
-      <c r="F63" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>240</v>
+        <v>131</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E64" t="s">
-        <v>599</v>
-      </c>
-      <c r="F64" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>501</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E65" t="s">
-        <v>240</v>
-      </c>
-      <c r="F65" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>215</v>
+        <v>143</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E66" t="s">
-        <v>131</v>
-      </c>
-      <c r="F66" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>126</v>
+        <v>324</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E67" t="s">
-        <v>215</v>
-      </c>
-      <c r="F67" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>91</v>
+        <v>384</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E68" t="s">
-        <v>126</v>
-      </c>
-      <c r="F68" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E69" t="s">
-        <v>91</v>
-      </c>
-      <c r="F69" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>281</v>
+        <v>551</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E70" t="s">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>615</v>
-      </c>
-      <c r="F70" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>575</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E71" t="s">
-        <v>281</v>
-      </c>
-      <c r="F71" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>226</v>
+        <v>559</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E72" t="s">
-        <v>575</v>
-      </c>
-      <c r="F72" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>239</v>
+        <v>392</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E73" t="s">
-        <v>226</v>
-      </c>
-      <c r="F73" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E74" t="s">
-        <v>239</v>
-      </c>
-      <c r="F74" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>633</v>
+        <v>449</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E75" t="s">
-        <v>100</v>
-      </c>
-      <c r="F75" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>609</v>
+        <v>573</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E76" t="s">
-        <v>633</v>
-      </c>
-      <c r="F76" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>560</v>
+        <v>511</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E77" t="s">
-        <v>609</v>
-      </c>
-      <c r="F77" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>324</v>
+        <v>15</v>
       </c>
       <c r="B78" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E78" t="s">
-        <v>560</v>
-      </c>
-      <c r="F78" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>171</v>
+        <v>398</v>
       </c>
       <c r="B79" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E79" t="s">
-        <v>324</v>
-      </c>
-      <c r="F79" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>234</v>
+        <v>575</v>
       </c>
       <c r="B80" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E80" t="s">
-        <v>171</v>
-      </c>
-      <c r="F80" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>254</v>
+        <v>12</v>
       </c>
       <c r="B81" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E81" t="s">
-        <v>234</v>
-      </c>
-      <c r="F81" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>286</v>
+        <v>462</v>
       </c>
       <c r="B82" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E82" t="s">
-        <v>254</v>
-      </c>
-      <c r="F82" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>513</v>
+        <v>114</v>
       </c>
       <c r="B83" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E83" t="s">
-        <v>286</v>
-      </c>
-      <c r="F83" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>202</v>
+        <v>537</v>
       </c>
       <c r="B84" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E84" t="s">
-        <v>513</v>
-      </c>
-      <c r="F84" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>227</v>
       </c>
       <c r="B85" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E85" t="s">
-        <v>202</v>
-      </c>
-      <c r="F85" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>456</v>
+        <v>613</v>
       </c>
       <c r="B86" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E86" t="s">
-        <v>90</v>
-      </c>
-      <c r="F86" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="B87" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E87" t="s">
-        <v>456</v>
-      </c>
-      <c r="F87" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>460</v>
+        <v>350</v>
       </c>
       <c r="B88" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E88" t="s">
-        <v>12</v>
-      </c>
-      <c r="F88" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="B89" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E89" t="s">
-        <v>460</v>
-      </c>
-      <c r="F89" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>204</v>
+        <v>599</v>
       </c>
       <c r="B90" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E90" t="s">
-        <v>172</v>
-      </c>
-      <c r="F90" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>263</v>
+        <v>400</v>
       </c>
       <c r="B91" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E91" t="s">
-        <v>204</v>
-      </c>
-      <c r="F91" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="B92" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E92" t="s">
-        <v>263</v>
-      </c>
-      <c r="F92" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>613</v>
+        <v>204</v>
       </c>
       <c r="B93" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E93" t="s">
-        <v>214</v>
-      </c>
-      <c r="F93" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>239</v>
       </c>
       <c r="B94" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E94" t="s">
-        <v>613</v>
-      </c>
-      <c r="F94" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>285</v>
+        <v>214</v>
       </c>
       <c r="B95" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E95" t="s">
-        <v>118</v>
-      </c>
-      <c r="F95" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>487</v>
+        <v>91</v>
       </c>
       <c r="B96" t="str">
         <f t="shared" si="1"/>
         <v>x</v>
       </c>
-      <c r="E96" t="s">
-        <v>285</v>
-      </c>
-      <c r="F96" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>296</v>
+        <v>90</v>
       </c>
       <c r="B97" t="str">
         <f t="shared" ref="B97:B160" si="2">IF(LEN(A97)=3, "x", " ")</f>
         <v>x</v>
       </c>
-      <c r="E97" t="s">
-        <v>487</v>
-      </c>
-      <c r="F97" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>416</v>
+        <v>171</v>
       </c>
       <c r="B98" t="str">
         <f t="shared" si="2"/>
         <v>x</v>
       </c>
-      <c r="E98" t="s">
-        <v>296</v>
-      </c>
-      <c r="F98" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>510</v>
+        <v>406</v>
       </c>
       <c r="B99" t="str">
         <f t="shared" si="2"/>
         <v>x</v>
       </c>
-      <c r="E99" t="s">
-        <v>416</v>
-      </c>
-      <c r="F99" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>350</v>
+        <v>456</v>
       </c>
       <c r="B100" t="str">
         <f t="shared" si="2"/>
         <v>x</v>
       </c>
-      <c r="E100" t="s">
-        <v>510</v>
-      </c>
-      <c r="F100" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B101" t="str">
         <f t="shared" si="2"/>
         <v>x</v>
       </c>
-      <c r="E101" t="s">
-        <v>350</v>
-      </c>
-      <c r="F101" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>500</v>
+      </c>
       <c r="B102" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E102" t="s">
-        <v>45</v>
-      </c>
-      <c r="F102" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>39</v>
+      </c>
       <c r="B103" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F103" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>383</v>
+      </c>
       <c r="B104" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F104" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>416</v>
+      </c>
       <c r="B105" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F105" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>189</v>
+      </c>
       <c r="B106" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F106" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>47</v>
+      </c>
       <c r="B107" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F107" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>296</v>
+      </c>
       <c r="B108" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F108" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>167</v>
+      </c>
       <c r="B109" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F109" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>612</v>
+      </c>
       <c r="B110" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F110" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>199</v>
+      </c>
       <c r="B111" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F111" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>309</v>
+      </c>
       <c r="B112" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F112" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F113" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F114" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F115" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F116" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F117" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F118" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F119" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F120" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F121" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F122" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F123" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F124" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F125" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F126" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F127" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F128" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F129" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F130" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F131" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F132" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F133" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F134" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F135" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F136" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F137" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F138" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F139" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F140" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F141" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F142" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F143" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B144" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F144" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F145" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F146" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F147" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F148" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F149" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F150" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F151" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F152" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F153" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F154" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F155" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F156" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F157" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F158" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F159" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F160" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" t="str">
         <f t="shared" ref="B161:B224" si="3">IF(LEN(A161)=3, "x", " ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F161" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F162" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F163" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F164" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F165" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F166" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F167" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F168" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F169" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F170" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F171" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F172" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F173" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F174" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F175" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F176" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F177" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F178" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F179" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F180" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F181" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F182" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F183" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F184" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F185" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F186" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F187" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F188" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F189" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F190" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F191" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F192" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F193" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F194" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F195" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F196" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F197" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F198" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F199" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F200" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F201" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F202" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F203" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F204" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F205" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F206" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F207" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F208" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F209" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F210" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F211" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F212" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B213" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F213" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B214" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F214" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B215" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F215" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B216" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F216" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B217" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F217" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B218" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F218" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B219" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F219" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B220" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F220" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B221" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F221" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B222" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F222" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B223" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F223" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B224" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F224" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B225" t="str">
         <f t="shared" ref="B225:B288" si="4">IF(LEN(A225)=3, "x", " ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F225" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B226" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F226" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B227" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F227" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B228" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F228" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="229" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B229" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F229" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B230" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F230" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="231" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B231" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F231" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="232" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B232" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F232" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B233" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F233" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B234" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F234" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="235" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B235" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F235" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="236" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B236" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F236" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="237" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B237" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F237" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="238" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B238" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F238" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="239" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B239" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F239" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B240" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F240" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="241" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B241" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F241" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="242" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B242" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F242" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="243" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B243" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F243" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="244" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B244" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F244" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="245" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B245" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F245" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="246" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B246" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F246" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="247" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B247" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F247" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="248" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B248" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F248" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="249" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B249" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F249" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="250" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B250" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F250" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="251" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B251" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F251" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="252" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B252" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F252" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="253" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B253" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F253" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="254" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B254" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F254" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="255" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B255" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F255" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="256" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B256" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F256" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="257" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B257" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F257" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="258" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B258" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F258" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="259" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B259" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B260" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B261" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B262" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B263" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B264" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B265" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B266" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B267" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B268" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B269" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B270" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B271" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B272" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>

</xml_diff>